<commit_message>
Added Label for Output
</commit_message>
<xml_diff>
--- a/SATS_final_output.xlsx
+++ b/SATS_final_output.xlsx
@@ -911,8 +911,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
         <v>8760</v>
@@ -1292,8 +1300,16 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>8760</v>
@@ -1725,8 +1741,16 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
         <v>7181</v>
@@ -2128,8 +2152,16 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
         <v>7181</v>
@@ -2529,8 +2561,16 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
         <v>1861</v>
@@ -2936,8 +2976,16 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
         <v>1861</v>
@@ -3341,8 +3389,16 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>6602</v>
@@ -3690,8 +3746,16 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>6602</v>
@@ -4095,8 +4159,16 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>9072</v>
@@ -4444,8 +4516,16 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>9072</v>
@@ -4793,8 +4873,16 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
         <v>6007</v>
@@ -5200,8 +5288,16 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>6007</v>
@@ -5603,8 +5699,16 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
         <v>3680</v>
@@ -6004,8 +6108,16 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
         <v>3680</v>

</xml_diff>